<commit_message>
Agregar script de análisis de impacto de energía renovable y archivos de resultados
</commit_message>
<xml_diff>
--- a/Predespacho/UC_datEx8.xlsx
+++ b/Predespacho/UC_datEx8.xlsx
@@ -5517,49 +5517,49 @@
         <v>-0.0</v>
       </c>
       <c r="J4">
+        <v>137.93361426858638</v>
+      </c>
+      <c r="K4">
         <v>40.0</v>
       </c>
-      <c r="K4">
-        <v>53.97300740615307</v>
-      </c>
       <c r="L4">
-        <v>103.17317056902215</v>
+        <v>54.58421351380747</v>
       </c>
       <c r="M4">
-        <v>135.86951697607986</v>
+        <v>93.66092801902477</v>
       </c>
       <c r="N4">
-        <v>126.58955573871503</v>
+        <v>106.46685635221195</v>
       </c>
       <c r="O4">
-        <v>82.59285304839233</v>
+        <v>82.59285304839221</v>
       </c>
       <c r="P4">
-        <v>48.27998673294732</v>
+        <v>40.0</v>
       </c>
       <c r="Q4">
         <v>40.0</v>
       </c>
       <c r="R4">
-        <v>40.0</v>
+        <v>172.59713278443235</v>
       </c>
       <c r="S4">
-        <v>-0.0</v>
+        <v>158.78497042674894</v>
       </c>
       <c r="T4">
-        <v>-0.0</v>
+        <v>106.74147800209144</v>
       </c>
       <c r="U4">
         <v>-0.0</v>
       </c>
       <c r="V4">
-        <v>139.96908374044145</v>
+        <v>-3.552713678800501e-14</v>
       </c>
       <c r="W4">
-        <v>64.57397239848035</v>
+        <v>64.57397239848032</v>
       </c>
       <c r="X4">
-        <v>59.44167376363205</v>
+        <v>59.44167376363208</v>
       </c>
       <c r="Y4">
         <v>40.0</v>
@@ -5597,10 +5597,10 @@
         <v>-0.0</v>
       </c>
       <c r="J5">
-        <v>101.36919709067213</v>
+        <v>-0.0</v>
       </c>
       <c r="K5">
-        <v>186.0</v>
+        <v>153.83803808099972</v>
       </c>
       <c r="L5">
         <v>186.0</v>
@@ -5615,25 +5615,25 @@
         <v>186.0</v>
       </c>
       <c r="P5">
-        <v>186.0</v>
+        <v>176.6112750765057</v>
       </c>
       <c r="Q5">
-        <v>178.57207932409239</v>
+        <v>178.08128177808024</v>
       </c>
       <c r="R5">
-        <v>127.68915732430963</v>
+        <v>-0.0</v>
       </c>
       <c r="S5">
-        <v>165.16533852490835</v>
+        <v>-0.0</v>
       </c>
       <c r="T5">
-        <v>116.06663137632447</v>
+        <v>-0.0</v>
       </c>
       <c r="U5">
         <v>-0.0</v>
       </c>
       <c r="V5">
-        <v>-0.0</v>
+        <v>139.96908374044148</v>
       </c>
       <c r="W5">
         <v>186.0</v>
@@ -5642,7 +5642,7 @@
         <v>186.0</v>
       </c>
       <c r="Y5">
-        <v>128.7685228668009</v>
+        <v>128.768522866801</v>
       </c>
       <c r="Z5">
         <v>51.654579955085794</v>
@@ -5659,49 +5659,49 @@
         <v>325.5</v>
       </c>
       <c r="D6">
-        <v>283.4495581136074</v>
+        <v>325.5</v>
       </c>
       <c r="E6">
-        <v>283.4664532097639</v>
+        <v>325.5</v>
       </c>
       <c r="F6">
-        <v>280.97743193320287</v>
+        <v>325.5</v>
       </c>
       <c r="G6">
         <v>325.5</v>
       </c>
       <c r="H6">
-        <v>277.47938957783276</v>
+        <v>276.1843038635469</v>
       </c>
       <c r="I6">
-        <v>290.7726300568261</v>
+        <v>287.96714434254034</v>
       </c>
       <c r="J6">
-        <v>210.8684403188663</v>
+        <v>284.36402840859375</v>
       </c>
       <c r="K6">
-        <v>133.54816555145095</v>
+        <v>144.36402840859375</v>
       </c>
       <c r="L6">
-        <v>88.28987574378863</v>
+        <v>107.27730431521715</v>
       </c>
       <c r="M6">
-        <v>192.76551242156603</v>
+        <v>222.77730431521715</v>
       </c>
       <c r="N6">
-        <v>64.80315661886607</v>
+        <v>210.0</v>
       </c>
       <c r="O6">
-        <v>86.60142471039438</v>
+        <v>325.5</v>
       </c>
       <c r="P6">
-        <v>122.96512430327701</v>
+        <v>325.5</v>
       </c>
       <c r="Q6">
-        <v>238.465124303277</v>
+        <v>213.00107246631615</v>
       </c>
       <c r="R6">
-        <v>315.56156565032313</v>
+        <v>158.12786803825804</v>
       </c>
       <c r="S6">
         <v>210.0</v>
@@ -5710,22 +5710,22 @@
         <v>325.5</v>
       </c>
       <c r="U6">
-        <v>325.5</v>
+        <v>288.7980398048054</v>
       </c>
       <c r="V6">
-        <v>210.34418381743637</v>
+        <v>205.17824096029358</v>
       </c>
       <c r="W6">
-        <v>146.32003878519987</v>
+        <v>141.00643878519986</v>
       </c>
       <c r="X6">
-        <v>261.82003878519987</v>
+        <v>137.30978151633713</v>
       </c>
       <c r="Y6">
-        <v>325.5</v>
+        <v>182.8787901873107</v>
       </c>
       <c r="Z6">
-        <v>325.5</v>
+        <v>298.3787901873107</v>
       </c>
     </row>
     <row r="7" spans="1:26" dyDescent="0.25">
@@ -5736,19 +5736,19 @@
         <v>51</v>
       </c>
       <c r="C7">
-        <v>299.5603965167394</v>
+        <v>245.94366508816802</v>
       </c>
       <c r="D7">
-        <v>325.5</v>
+        <v>213.68864382789315</v>
       </c>
       <c r="E7">
-        <v>325.5</v>
+        <v>223.5773103526211</v>
       </c>
       <c r="F7">
-        <v>325.5</v>
+        <v>255.85155764748868</v>
       </c>
       <c r="G7">
-        <v>275.5573634394343</v>
+        <v>268.69999201086307</v>
       </c>
       <c r="H7">
         <v>325.5</v>
@@ -5757,7 +5757,7 @@
         <v>325.5</v>
       </c>
       <c r="J7">
-        <v>325.5</v>
+        <v>251.57858333884383</v>
       </c>
       <c r="K7">
         <v>325.5</v>
@@ -5766,31 +5766,31 @@
         <v>325.5</v>
       </c>
       <c r="M7">
-        <v>210.0</v>
+        <v>187.61723667777738</v>
       </c>
       <c r="N7">
+        <v>195.8674994760089</v>
+      </c>
+      <c r="O7">
+        <v>96.15845328182303</v>
+      </c>
+      <c r="P7">
+        <v>135.12718144613407</v>
+      </c>
+      <c r="Q7">
+        <v>250.62718144613405</v>
+      </c>
+      <c r="R7">
         <v>325.5</v>
       </c>
-      <c r="O7">
+      <c r="S7">
+        <v>280.07373095936333</v>
+      </c>
+      <c r="T7">
+        <v>217.40045780001805</v>
+      </c>
+      <c r="U7">
         <v>325.5</v>
-      </c>
-      <c r="P7">
-        <v>325.5</v>
-      </c>
-      <c r="Q7">
-        <v>214.12015818060192</v>
-      </c>
-      <c r="R7">
-        <v>159.80435953079206</v>
-      </c>
-      <c r="S7">
-        <v>275.30435953079206</v>
-      </c>
-      <c r="T7">
-        <v>218.6459435143039</v>
-      </c>
-      <c r="U7">
-        <v>267.68581123337685</v>
       </c>
       <c r="V7">
         <v>325.5</v>
@@ -5799,13 +5799,13 @@
         <v>325.5</v>
       </c>
       <c r="X7">
-        <v>215.895228445423</v>
+        <v>325.5</v>
       </c>
       <c r="Y7">
-        <v>199.46279018731076</v>
+        <v>325.5</v>
       </c>
       <c r="Z7">
-        <v>246.59262690408974</v>
+        <v>264.1677795739219</v>
       </c>
     </row>
     <row r="8" spans="1:26" dyDescent="0.25">
@@ -5822,7 +5822,7 @@
         <v>8.0</v>
       </c>
       <c r="E8">
-        <v>9.659441083653052</v>
+        <v>-0.0</v>
       </c>
       <c r="F8">
         <v>-0.0</v>
@@ -5834,7 +5834,7 @@
         <v>-0.0</v>
       </c>
       <c r="I8">
-        <v>8.0</v>
+        <v>-0.0</v>
       </c>
       <c r="J8">
         <v>18.6</v>
@@ -5914,7 +5914,7 @@
         <v>-0.0</v>
       </c>
       <c r="I9">
-        <v>8.845217522251943</v>
+        <v>8.0</v>
       </c>
       <c r="J9">
         <v>18.6</v>
@@ -5950,7 +5950,7 @@
         <v>18.6</v>
       </c>
       <c r="U9">
-        <v>17.354984873298356</v>
+        <v>17.35498487329827</v>
       </c>
       <c r="V9">
         <v>18.6</v>
@@ -5991,10 +5991,10 @@
         <v>-0.0</v>
       </c>
       <c r="H10">
-        <v>8.0</v>
+        <v>-0.0</v>
       </c>
       <c r="I10">
-        <v>18.6</v>
+        <v>8.845217522253215</v>
       </c>
       <c r="J10">
         <v>18.6</v>
@@ -6062,7 +6062,7 @@
         <v>8.0</v>
       </c>
       <c r="E11">
-        <v>-0.0</v>
+        <v>9.65944108365268</v>
       </c>
       <c r="F11">
         <v>-0.0</v>
@@ -6071,10 +6071,10 @@
         <v>-0.0</v>
       </c>
       <c r="H11">
-        <v>-0.0</v>
+        <v>5.806585797609421e-14</v>
       </c>
       <c r="I11">
-        <v>18.6</v>
+        <v>18.600000000000136</v>
       </c>
       <c r="J11">
         <v>18.6</v>
@@ -6142,7 +6142,7 @@
         <v>8.0</v>
       </c>
       <c r="E12">
-        <v>-4.4231285301066237e-13</v>
+        <v>-0.0</v>
       </c>
       <c r="F12">
         <v>-0.0</v>
@@ -6151,10 +6151,10 @@
         <v>-0.0</v>
       </c>
       <c r="H12">
-        <v>-0.0</v>
+        <v>8.0</v>
       </c>
       <c r="I12">
-        <v>1.4050982599655981e-12</v>
+        <v>18.6</v>
       </c>
       <c r="J12">
         <v>18.6</v>
@@ -6237,37 +6237,37 @@
         <v>-0.0</v>
       </c>
       <c r="J13">
-        <v>3.9263803680981595</v>
+        <v>7.361963190184049</v>
       </c>
       <c r="K13">
-        <v>15.705521472392638</v>
+        <v>61.84049079754601</v>
       </c>
       <c r="L13">
-        <v>30.429447852760735</v>
+        <v>79.01840490797547</v>
       </c>
       <c r="M13">
-        <v>34.355828220858896</v>
+        <v>76.56441717791411</v>
       </c>
       <c r="N13">
-        <v>51.04294478527607</v>
+        <v>71.16564417177914</v>
       </c>
       <c r="O13">
         <v>69.20245398773005</v>
       </c>
       <c r="P13">
-        <v>39.75460122699386</v>
+        <v>57.42331288343558</v>
       </c>
       <c r="Q13">
-        <v>50.5521472392638</v>
+        <v>51.04294478527607</v>
       </c>
       <c r="R13">
-        <v>68.71165644171779</v>
+        <v>63.803680981595086</v>
       </c>
       <c r="S13">
-        <v>54.96932515337423</v>
+        <v>61.34969325153374</v>
       </c>
       <c r="T13">
-        <v>7.361963190184049</v>
+        <v>16.68711656441718</v>
       </c>
       <c r="U13">
         <v>-0.0</v>
@@ -6296,76 +6296,76 @@
         <v>52</v>
       </c>
       <c r="C14">
-        <v>0.6849828571428572</v>
+        <v>54.30171428571428</v>
       </c>
       <c r="D14">
-        <v>4.970514285714286</v>
+        <v>74.73142857142858</v>
       </c>
       <c r="E14">
-        <v>2.8674285714285714</v>
+        <v>62.75657142857143</v>
       </c>
       <c r="F14">
-        <v>2.0284114285714288</v>
+        <v>27.154285714285717</v>
       </c>
       <c r="G14">
-        <v>6.287085714285714</v>
+        <v>13.144457142857142</v>
       </c>
       <c r="H14">
-        <v>8.1456</v>
+        <v>9.440685714285715</v>
       </c>
       <c r="I14">
-        <v>4.229257142857143</v>
+        <v>7.034742857142858</v>
       </c>
       <c r="J14">
-        <v>2.940342857142857</v>
+        <v>3.3661714285714286</v>
       </c>
       <c r="K14">
-        <v>12.797714285714285</v>
+        <v>1.9818514285714286</v>
       </c>
       <c r="L14">
-        <v>18.987428571428573</v>
+        <v>-0.0</v>
       </c>
       <c r="M14">
-        <v>7.629028571428571</v>
+        <v>-0.0</v>
       </c>
       <c r="N14">
-        <v>15.564342857142856</v>
+        <v>-0.0</v>
       </c>
       <c r="O14">
-        <v>9.557028571428571</v>
+        <v>-0.0</v>
       </c>
       <c r="P14">
-        <v>12.162057142857144</v>
+        <v>-0.0</v>
       </c>
       <c r="Q14">
-        <v>11.042971428571429</v>
+        <v>-0.0</v>
       </c>
       <c r="R14">
-        <v>8.261942857142856</v>
+        <v>-0.0</v>
       </c>
       <c r="S14">
-        <v>8.264914285714285</v>
+        <v>3.4955428571428575</v>
       </c>
       <c r="T14">
-        <v>8.527314285714287</v>
+        <v>9.7728</v>
       </c>
       <c r="U14">
-        <v>32.61028571428571</v>
+        <v>11.498057142857142</v>
       </c>
       <c r="V14">
-        <v>6.720000000000001</v>
+        <v>11.885942857142858</v>
       </c>
       <c r="W14">
-        <v>3.1456</v>
+        <v>8.4592</v>
       </c>
       <c r="X14">
-        <v>0.38708571428571426</v>
+        <v>15.292571428571428</v>
       </c>
       <c r="Y14">
-        <v>-0.0</v>
+        <v>16.584</v>
       </c>
       <c r="Z14">
-        <v>-0.0</v>
+        <v>9.546057142857142</v>
       </c>
     </row>
   </sheetData>
@@ -6550,16 +6550,16 @@
         <v>14.000000000000002</v>
       </c>
       <c r="S4">
-        <v>-0.0</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="T4">
-        <v>-0.0</v>
+        <v>14.000000000000014</v>
       </c>
       <c r="U4">
         <v>-0.0</v>
       </c>
       <c r="V4">
-        <v>14.000000000000002</v>
+        <v>-0.0</v>
       </c>
       <c r="W4">
         <v>14.000000000000002</v>
@@ -6603,7 +6603,7 @@
         <v>-0.0</v>
       </c>
       <c r="J5">
-        <v>14.000000000000002</v>
+        <v>-0.0</v>
       </c>
       <c r="K5">
         <v>14.000000000000002</v>
@@ -6624,22 +6624,22 @@
         <v>14.000000000000002</v>
       </c>
       <c r="Q5">
+        <v>13.999999999999934</v>
+      </c>
+      <c r="R5">
+        <v>-0.0</v>
+      </c>
+      <c r="S5">
+        <v>-0.0</v>
+      </c>
+      <c r="T5">
+        <v>-0.0</v>
+      </c>
+      <c r="U5">
+        <v>-0.0</v>
+      </c>
+      <c r="V5">
         <v>14.000000000000002</v>
-      </c>
-      <c r="R5">
-        <v>14.000000000000002</v>
-      </c>
-      <c r="S5">
-        <v>14.000000000000002</v>
-      </c>
-      <c r="T5">
-        <v>14.000000000000002</v>
-      </c>
-      <c r="U5">
-        <v>-0.0</v>
-      </c>
-      <c r="V5">
-        <v>-0.0</v>
       </c>
       <c r="W5">
         <v>14.000000000000002</v>
@@ -6828,7 +6828,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="E8">
-        <v>1.4000000000000001</v>
+        <v>-0.0</v>
       </c>
       <c r="F8">
         <v>-0.0</v>
@@ -6840,7 +6840,7 @@
         <v>-0.0</v>
       </c>
       <c r="I8">
-        <v>1.4000000000000001</v>
+        <v>-0.0</v>
       </c>
       <c r="J8">
         <v>1.4000000000000001</v>
@@ -6920,7 +6920,7 @@
         <v>-0.0</v>
       </c>
       <c r="I9">
-        <v>1.399999999989346</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="J9">
         <v>1.4000000000000001</v>
@@ -6997,7 +6997,7 @@
         <v>-0.0</v>
       </c>
       <c r="H10">
-        <v>1.4000000000000001</v>
+        <v>-0.0</v>
       </c>
       <c r="I10">
         <v>1.4000000000000001</v>
@@ -7068,7 +7068,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="E11">
-        <v>-0.0</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="F11">
         <v>-0.0</v>
@@ -7077,10 +7077,10 @@
         <v>-0.0</v>
       </c>
       <c r="H11">
-        <v>-0.0</v>
+        <v>1.0161525145816487e-14</v>
       </c>
       <c r="I11">
-        <v>1.4000000000000001</v>
+        <v>1.4000000000000103</v>
       </c>
       <c r="J11">
         <v>1.4000000000000001</v>
@@ -7148,7 +7148,7 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="E12">
-        <v>-7.740474927686592e-14</v>
+        <v>-0.0</v>
       </c>
       <c r="F12">
         <v>-0.0</v>
@@ -7157,10 +7157,10 @@
         <v>-0.0</v>
       </c>
       <c r="H12">
-        <v>-0.0</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="I12">
-        <v>2.458921954939797e-13</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="J12">
         <v>1.4000000000000001</v>
@@ -7526,64 +7526,64 @@
         <v>139.13174000816372</v>
       </c>
       <c r="H4">
-        <v>138.74048311274103</v>
+        <v>138.740483112741</v>
       </c>
       <c r="I4">
-        <v>138.47568303683764</v>
+        <v>138.47568303683775</v>
       </c>
       <c r="J4">
-        <v>139.03325305137483</v>
+        <v>139.03325305137474</v>
       </c>
       <c r="K4">
         <v>139.4191808900948</v>
       </c>
       <c r="L4">
-        <v>41.94678528896516</v>
+        <v>41.946785288965046</v>
       </c>
       <c r="M4">
-        <v>-32.295921869017945</v>
+        <v>-32.295921869017974</v>
       </c>
       <c r="N4">
-        <v>-75.2907630039598</v>
+        <v>-75.29076300395985</v>
       </c>
       <c r="O4">
-        <v>-99.92292172342317</v>
+        <v>-99.92292172342326</v>
       </c>
       <c r="P4">
         <v>-104.90491628641257</v>
       </c>
       <c r="Q4">
-        <v>-87.52702264222862</v>
+        <v>-87.52702264222853</v>
       </c>
       <c r="R4">
-        <v>-44.64206320176847</v>
+        <v>-44.642063201768565</v>
       </c>
       <c r="S4">
-        <v>-41.339392648775714</v>
+        <v>-41.33939264877577</v>
       </c>
       <c r="T4">
         <v>-19.329881920231884</v>
       </c>
       <c r="U4">
-        <v>-8.3893969810342</v>
+        <v>-8.38939698103432</v>
       </c>
       <c r="V4">
-        <v>56.65434643330296</v>
+        <v>56.65434643330289</v>
       </c>
       <c r="W4">
-        <v>139.59474288453475</v>
+        <v>139.5947428845348</v>
       </c>
       <c r="X4">
         <v>45.52934317695687</v>
       </c>
       <c r="Y4">
-        <v>-28.862637226359084</v>
+        <v>-28.862637226359055</v>
       </c>
       <c r="Z4">
-        <v>-25.41069342803357</v>
+        <v>-25.410693428033596</v>
       </c>
       <c r="AA4">
-        <v>26.15906635548198</v>
+        <v>26.15906635548191</v>
       </c>
       <c r="AB4">
         <v>78.02529939014438</v>
@@ -7612,19 +7612,19 @@
         <v>139.13174000816372</v>
       </c>
       <c r="H5">
-        <v>138.74048311274103</v>
+        <v>138.740483112741</v>
       </c>
       <c r="I5">
-        <v>138.47568303683764</v>
+        <v>138.47568303683775</v>
       </c>
       <c r="J5">
-        <v>139.03325305137483</v>
+        <v>139.03325305137474</v>
       </c>
       <c r="K5">
         <v>139.4191808900948</v>
       </c>
       <c r="L5">
-        <v>187.24236274773546</v>
+        <v>187.24236274773548</v>
       </c>
       <c r="M5">
         <v>223.38260700952776</v>
@@ -7633,19 +7633,19 @@
         <v>244.3118554178231</v>
       </c>
       <c r="O5">
-        <v>256.30242347351555</v>
+        <v>256.3024234735156</v>
       </c>
       <c r="P5">
         <v>258.7275842375785</v>
       </c>
       <c r="Q5">
-        <v>250.2682843938938</v>
+        <v>250.26828439389377</v>
       </c>
       <c r="R5">
         <v>229.39252475817273</v>
       </c>
       <c r="S5">
-        <v>227.78483391458047</v>
+        <v>227.78483391458053</v>
       </c>
       <c r="T5">
         <v>217.07093184579554</v>
@@ -7654,10 +7654,10 @@
         <v>211.74526669724838</v>
       </c>
       <c r="V5">
-        <v>180.08294099981148</v>
+        <v>180.0829409998115</v>
       </c>
       <c r="W5">
-        <v>139.59474288453475</v>
+        <v>139.5947428845348</v>
       </c>
       <c r="X5">
         <v>185.49842691739832</v>
@@ -7669,7 +7669,7 @@
         <v>220.03098033559849</v>
       </c>
       <c r="AA5">
-        <v>194.92758922228288</v>
+        <v>194.9275892222829</v>
       </c>
       <c r="AB5">
         <v>169.67987934523018</v>
@@ -7698,10 +7698,10 @@
         <v>300.0</v>
       </c>
       <c r="H6">
-        <v>299.29092273206624</v>
+        <v>299.29092273206635</v>
       </c>
       <c r="I6">
-        <v>298.71969609886935</v>
+        <v>298.71969609886946</v>
       </c>
       <c r="J6">
         <v>299.8107262904728</v>
@@ -7775,7 +7775,7 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>145.18764254044797</v>
+        <v>145.187642540448</v>
       </c>
       <c r="F7">
         <v>139.44689906340875</v>
@@ -7784,10 +7784,10 @@
         <v>136.6735433460813</v>
       </c>
       <c r="H7">
-        <v>135.19873645251627</v>
+        <v>135.1987364525163</v>
       </c>
       <c r="I7">
-        <v>134.94069615402924</v>
+        <v>134.94069615402918</v>
       </c>
       <c r="J7">
         <v>136.3897064923426</v>
@@ -7796,13 +7796,13 @@
         <v>141.978526325708</v>
       </c>
       <c r="L7">
-        <v>152.28348422705676</v>
+        <v>152.28348422705673</v>
       </c>
       <c r="M7">
         <v>156.57516931686658</v>
       </c>
       <c r="N7">
-        <v>159.0605355663074</v>
+        <v>159.06053556630744</v>
       </c>
       <c r="O7">
         <v>160.48442583584193</v>
@@ -7817,7 +7817,7 @@
         <v>157.28885221856493</v>
       </c>
       <c r="S7">
-        <v>157.0979375481358</v>
+        <v>157.09793754813577</v>
       </c>
       <c r="T7">
         <v>155.82565246258926</v>
@@ -7826,16 +7826,16 @@
         <v>155.1932251456687</v>
       </c>
       <c r="V7">
-        <v>151.4332967367716</v>
+        <v>151.43329673677158</v>
       </c>
       <c r="W7">
-        <v>145.218682653217</v>
+        <v>145.21868265321703</v>
       </c>
       <c r="X7">
         <v>152.07639034726924</v>
       </c>
       <c r="Y7">
-        <v>156.3767043487369</v>
+        <v>156.37670434873687</v>
       </c>
       <c r="Z7">
         <v>156.17716076664993</v>
@@ -7861,7 +7861,7 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>93.9817977890514</v>
+        <v>93.98179778905141</v>
       </c>
       <c r="F8">
         <v>92.06138657070429</v>
@@ -7870,10 +7870,10 @@
         <v>91.63779531239685</v>
       </c>
       <c r="H8">
-        <v>91.10411012195291</v>
+        <v>91.10411012195294</v>
       </c>
       <c r="I8">
-        <v>90.93022882404952</v>
+        <v>90.9302288240495</v>
       </c>
       <c r="J8">
         <v>91.52557681278951</v>
@@ -7882,13 +7882,13 @@
         <v>93.09830134585752</v>
       </c>
       <c r="L8">
-        <v>95.93534215207275</v>
+        <v>95.93534215207272</v>
       </c>
       <c r="M8">
         <v>97.11687883022086</v>
       </c>
       <c r="N8">
-        <v>97.80112087522046</v>
+        <v>97.80112087522048</v>
       </c>
       <c r="O8">
         <v>98.19312973512211</v>
@@ -7903,25 +7903,25 @@
         <v>97.31336168189279</v>
       </c>
       <c r="S8">
-        <v>97.260801281773</v>
+        <v>97.26080128177298</v>
       </c>
       <c r="T8">
         <v>96.9105305927135</v>
       </c>
       <c r="U8">
-        <v>96.73641808082893</v>
+        <v>96.73641808082891</v>
       </c>
       <c r="V8">
-        <v>95.70127844934214</v>
+        <v>95.70127844934211</v>
       </c>
       <c r="W8">
-        <v>93.99034339082854</v>
+        <v>93.99034339082856</v>
       </c>
       <c r="X8">
         <v>95.87832748075635</v>
       </c>
       <c r="Y8">
-        <v>97.06223977020933</v>
+        <v>97.06223977020932</v>
       </c>
       <c r="Z8">
         <v>97.00730375878467</v>
@@ -7947,7 +7947,7 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>73.49945988849277</v>
+        <v>73.49945988849278</v>
       </c>
       <c r="F9">
         <v>73.1071815736225</v>
@@ -7956,10 +7956,10 @@
         <v>73.62349609892307</v>
       </c>
       <c r="H9">
-        <v>73.46625958972757</v>
+        <v>73.4662595897276</v>
       </c>
       <c r="I9">
-        <v>73.32604189205763</v>
+        <v>73.3260418920576</v>
       </c>
       <c r="J9">
         <v>73.57992494096827</v>
@@ -7968,16 +7968,16 @@
         <v>73.54621135391733</v>
       </c>
       <c r="L9">
-        <v>73.39608532207914</v>
+        <v>73.39608532207912</v>
       </c>
       <c r="M9">
         <v>73.33356263556257</v>
       </c>
       <c r="N9">
-        <v>73.29735499878568</v>
+        <v>73.29735499878569</v>
       </c>
       <c r="O9">
-        <v>73.2766112948342</v>
+        <v>73.27661129483418</v>
       </c>
       <c r="P9">
         <v>73.27241576242146</v>
@@ -7989,25 +7989,25 @@
         <v>73.32316546722394</v>
       </c>
       <c r="S9">
-        <v>73.32594677522789</v>
+        <v>73.32594677522786</v>
       </c>
       <c r="T9">
         <v>73.3444818447632</v>
       </c>
       <c r="U9">
-        <v>73.35369525489301</v>
+        <v>73.353695254893</v>
       </c>
       <c r="V9">
-        <v>73.40847113437034</v>
+        <v>73.40847113437033</v>
       </c>
       <c r="W9">
-        <v>73.49900768587315</v>
+        <v>73.49900768587317</v>
       </c>
       <c r="X9">
         <v>73.3991023341512</v>
       </c>
       <c r="Y9">
-        <v>73.33645393879831</v>
+        <v>73.3364539387983</v>
       </c>
       <c r="Z9">
         <v>73.33936095563857</v>
@@ -8033,73 +8033,73 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>-8.42989171374177</v>
+        <v>-8.429891713741757</v>
       </c>
       <c r="F10">
         <v>-2.709638414704663</v>
       </c>
       <c r="G10">
-        <v>1.566299245027973</v>
+        <v>1.566299245027977</v>
       </c>
       <c r="H10">
-        <v>2.9148574608262123</v>
+        <v>2.914857460826238</v>
       </c>
       <c r="I10">
-        <v>2.9092941640900922</v>
+        <v>2.909294164090075</v>
       </c>
       <c r="J10">
-        <v>1.7973174536833056</v>
+        <v>1.7973174536833012</v>
       </c>
       <c r="K10">
         <v>-4.662148613843427</v>
       </c>
       <c r="L10">
-        <v>-16.760941997895287</v>
+        <v>-16.760941997895312</v>
       </c>
       <c r="M10">
-        <v>-21.79970214307059</v>
+        <v>-21.799702143070586</v>
       </c>
       <c r="N10">
-        <v>-24.717708506953468</v>
+        <v>-24.717708506953457</v>
       </c>
       <c r="O10">
-        <v>-26.389462466317497</v>
+        <v>-26.389462466317507</v>
       </c>
       <c r="P10">
         <v>-26.727584237578537</v>
       </c>
       <c r="Q10">
-        <v>-25.548168221469627</v>
+        <v>-25.54816822146962</v>
       </c>
       <c r="R10">
-        <v>-22.63761939145145</v>
+        <v>-22.637619391451455</v>
       </c>
       <c r="S10">
-        <v>-22.41347125095257</v>
+        <v>-22.413471250952593</v>
       </c>
       <c r="T10">
         <v>-20.919713147038014</v>
       </c>
       <c r="U10">
-        <v>-20.177196048850632</v>
+        <v>-20.177196048850647</v>
       </c>
       <c r="V10">
-        <v>-15.762758125516813</v>
+        <v>-15.762758125516818</v>
       </c>
       <c r="W10">
-        <v>-8.466335133948391</v>
+        <v>-8.466335133948382</v>
       </c>
       <c r="X10">
         <v>-16.517798252269436</v>
       </c>
       <c r="Y10">
-        <v>-21.566689386845773</v>
+        <v>-21.566689386845777</v>
       </c>
       <c r="Z10">
-        <v>-21.33241025694586</v>
+        <v>-21.332410256945856</v>
       </c>
       <c r="AA10">
-        <v>-17.83243483524545</v>
+        <v>-17.832434835245447</v>
       </c>
       <c r="AB10">
         <v>-14.31233814292907</v>
@@ -8125,16 +8125,16 @@
         <v>46.56779669741255</v>
       </c>
       <c r="G11">
-        <v>35.01902539460039</v>
+        <v>35.019025394600426</v>
       </c>
       <c r="H11">
-        <v>31.205665109790036</v>
+        <v>31.20566510979004</v>
       </c>
       <c r="I11">
-        <v>31.146105979647935</v>
+        <v>31.146105979647974</v>
       </c>
       <c r="J11">
-        <v>34.35687666262528</v>
+        <v>34.356876662625275</v>
       </c>
       <c r="K11">
         <v>52.201947141134085</v>
@@ -8143,49 +8143,49 @@
         <v>85.5798648272449</v>
       </c>
       <c r="M11">
-        <v>99.4806990697247</v>
+        <v>99.48069906972468</v>
       </c>
       <c r="N11">
-        <v>107.53083871006393</v>
+        <v>107.53083871006395</v>
       </c>
       <c r="O11">
-        <v>112.14284126898323</v>
+        <v>112.14284126898325</v>
       </c>
       <c r="P11">
         <v>113.07564508592493</v>
       </c>
       <c r="Q11">
-        <v>109.82189494293503</v>
+        <v>109.82189494293502</v>
       </c>
       <c r="R11">
-        <v>101.7923290030944</v>
+        <v>101.79232900309438</v>
       </c>
       <c r="S11">
-        <v>101.1739534390544</v>
+        <v>101.17395343905443</v>
       </c>
       <c r="T11">
         <v>97.0530024109012</v>
       </c>
       <c r="U11">
-        <v>95.00456057070116</v>
+        <v>95.00456057070112</v>
       </c>
       <c r="V11">
-        <v>82.8260944246715</v>
+        <v>82.82609442467154</v>
       </c>
       <c r="W11">
-        <v>62.69686349354083</v>
+        <v>62.69686349354077</v>
       </c>
       <c r="X11">
         <v>84.90908455438807</v>
       </c>
       <c r="Y11">
-        <v>98.83786797490353</v>
+        <v>98.83786797490355</v>
       </c>
       <c r="Z11">
         <v>98.19154323282793</v>
       </c>
       <c r="AA11">
-        <v>88.53587858754878</v>
+        <v>88.5358785875488</v>
       </c>
       <c r="AB11">
         <v>78.82470376922662</v>
@@ -8211,28 +8211,28 @@
         <v>69.86707169978285</v>
       </c>
       <c r="G12">
-        <v>71.5004706412142</v>
+        <v>71.50047064121425</v>
       </c>
       <c r="H12">
-        <v>71.70658062273577</v>
+        <v>71.70658062273579</v>
       </c>
       <c r="I12">
-        <v>71.5697214482133</v>
+        <v>71.56972144821326</v>
       </c>
       <c r="J12">
-        <v>71.51971711461883</v>
+        <v>71.51971711461886</v>
       </c>
       <c r="K12">
         <v>69.77274142435046</v>
       </c>
       <c r="L12">
-        <v>66.416618150612</v>
+        <v>66.41661815061204</v>
       </c>
       <c r="M12">
         <v>65.01890024129561</v>
       </c>
       <c r="N12">
-        <v>64.20946505549823</v>
+        <v>64.20946505549821</v>
       </c>
       <c r="O12">
         <v>63.74573183906182</v>
@@ -8244,7 +8244,7 @@
         <v>63.97910115991639</v>
       </c>
       <c r="R12">
-        <v>64.78646767637014</v>
+        <v>64.78646767637018</v>
       </c>
       <c r="S12">
         <v>64.84864485116887</v>
@@ -8253,25 +8253,25 @@
         <v>65.26300322383861</v>
       </c>
       <c r="U12">
-        <v>65.4689724337649</v>
+        <v>65.46897243376497</v>
       </c>
       <c r="V12">
-        <v>66.69350759067602</v>
+        <v>66.693507590676</v>
       </c>
       <c r="W12">
-        <v>68.71748587013991</v>
+        <v>68.71748587013995</v>
       </c>
       <c r="X12">
         <v>66.4840645775123</v>
       </c>
       <c r="Y12">
-        <v>65.08353640040838</v>
+        <v>65.08353640040836</v>
       </c>
       <c r="Z12">
-        <v>65.14852384299456</v>
+        <v>65.14852384299455</v>
       </c>
       <c r="AA12">
-        <v>66.11939330058564</v>
+        <v>66.11939330058566</v>
       </c>
       <c r="AB12">
         <v>67.09584426225473</v>
@@ -8300,52 +8300,52 @@
         <v>4.982653699626468</v>
       </c>
       <c r="H13">
-        <v>2.362321145061685</v>
+        <v>2.362321145061707</v>
       </c>
       <c r="I13">
-        <v>2.357812419097428</v>
+        <v>2.3578124190973244</v>
       </c>
       <c r="J13">
-        <v>4.531961923195098</v>
+        <v>4.5319619231951975</v>
       </c>
       <c r="K13">
         <v>16.99753904542672</v>
       </c>
       <c r="L13">
-        <v>-6.928308107786586</v>
+        <v>-6.92830810778662</v>
       </c>
       <c r="M13">
-        <v>-33.11607745226145</v>
+        <v>-33.116077452261436</v>
       </c>
       <c r="N13">
         <v>-48.28172840634478</v>
       </c>
       <c r="O13">
-        <v>-56.97027595121219</v>
+        <v>-56.9702759512122</v>
       </c>
       <c r="P13">
         <v>-58.72758423757853</v>
       </c>
       <c r="Q13">
-        <v>-52.597847218718066</v>
+        <v>-52.59784721871805</v>
       </c>
       <c r="R13">
-        <v>-37.47095504082192</v>
+        <v>-37.470955040821934</v>
       </c>
       <c r="S13">
-        <v>-36.30599786221957</v>
+        <v>-36.3059978622196</v>
       </c>
       <c r="T13">
         <v>-28.54254186219312</v>
       </c>
       <c r="U13">
-        <v>-24.68348408976109</v>
+        <v>-24.68348408976111</v>
       </c>
       <c r="V13">
-        <v>-1.7404824800371728</v>
+        <v>-1.7404824800372012</v>
       </c>
       <c r="W13">
-        <v>24.335942755108334</v>
+        <v>24.335942755108277</v>
       </c>
       <c r="X13">
         <v>-5.664625744557085</v>
@@ -8354,10 +8354,10 @@
         <v>-31.90504852083312</v>
       </c>
       <c r="Z13">
-        <v>-30.687437910429626</v>
+        <v>-30.687437910429622</v>
       </c>
       <c r="AA13">
-        <v>-12.497139818430902</v>
+        <v>-12.497139818430924</v>
       </c>
       <c r="AB13">
         <v>5.797733839506165</v>
@@ -8383,28 +8383,28 @@
         <v>-38.7027058584939</v>
       </c>
       <c r="G14">
-        <v>-48.356537224048026</v>
+        <v>-48.35653722404798</v>
       </c>
       <c r="H14">
-        <v>-51.20583678707706</v>
+        <v>-51.20583678707708</v>
       </c>
       <c r="I14">
-        <v>-51.108105330737246</v>
+        <v>-51.108105330737175</v>
       </c>
       <c r="J14">
-        <v>-48.83449045764162</v>
+        <v>-48.83449045764166</v>
       </c>
       <c r="K14">
         <v>-34.706358656247644</v>
       </c>
       <c r="L14">
-        <v>-8.190813549451931</v>
+        <v>-8.190813549451889</v>
       </c>
       <c r="M14">
         <v>2.8520621878784738</v>
       </c>
       <c r="N14">
-        <v>9.247123819846067</v>
+        <v>9.247123819846053</v>
       </c>
       <c r="O14">
         <v>12.910916241941038</v>
@@ -8416,7 +8416,7 @@
         <v>11.067147628886069</v>
       </c>
       <c r="R14">
-        <v>4.688429823058669</v>
+        <v>4.688429823058712</v>
       </c>
       <c r="S14">
         <v>4.1971899166200615</v>
@@ -8425,25 +8425,25 @@
         <v>0.9234907033416277</v>
       </c>
       <c r="U14">
-        <v>-0.7037993068759789</v>
+        <v>-0.7037993068759079</v>
       </c>
       <c r="V14">
-        <v>-10.378419259606105</v>
+        <v>-10.378419259606119</v>
       </c>
       <c r="W14">
-        <v>-26.369157080306195</v>
+        <v>-26.369157080306152</v>
       </c>
       <c r="X14">
         <v>-8.723683956436133</v>
       </c>
       <c r="Y14">
-        <v>2.3413947145185716</v>
+        <v>2.3413947145185574</v>
       </c>
       <c r="Z14">
-        <v>1.8279518744556071</v>
+        <v>1.827951874455593</v>
       </c>
       <c r="AA14">
-        <v>-5.842544944599382</v>
+        <v>-5.842544944599368</v>
       </c>
       <c r="AB14">
         <v>-13.557139256824826</v>
@@ -8682,16 +8682,16 @@
         <v>1.0</v>
       </c>
       <c r="S4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="T4">
-        <v>0.0</v>
+        <v>1.0000000000000009</v>
       </c>
       <c r="U4">
         <v>0.0</v>
       </c>
       <c r="V4">
-        <v>1.0</v>
+        <v>-8.881784197001252e-16</v>
       </c>
       <c r="W4">
         <v>1.0</v>
@@ -8735,7 +8735,7 @@
         <v>0.0</v>
       </c>
       <c r="J5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K5">
         <v>1.0</v>
@@ -8756,22 +8756,22 @@
         <v>1.0</v>
       </c>
       <c r="Q5">
-        <v>1.0</v>
+        <v>0.9999999999999952</v>
       </c>
       <c r="R5">
-        <v>1.0</v>
+        <v>-2.2204460492503446e-17</v>
       </c>
       <c r="S5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="T5">
-        <v>1.0</v>
+        <v>-0.0</v>
       </c>
       <c r="U5">
         <v>0.0</v>
       </c>
       <c r="V5">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="W5">
         <v>1.0</v>
@@ -8960,7 +8960,7 @@
         <v>1.0</v>
       </c>
       <c r="E8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F8">
         <v>0.0</v>
@@ -8972,7 +8972,7 @@
         <v>0.0</v>
       </c>
       <c r="I8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J8">
         <v>1.0</v>
@@ -9052,7 +9052,7 @@
         <v>0.0</v>
       </c>
       <c r="I9">
-        <v>0.9999999999923899</v>
+        <v>1.0</v>
       </c>
       <c r="J9">
         <v>1.0</v>
@@ -9129,7 +9129,7 @@
         <v>0.0</v>
       </c>
       <c r="H10">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I10">
         <v>1.0</v>
@@ -9200,7 +9200,7 @@
         <v>1.0</v>
       </c>
       <c r="E11">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F11">
         <v>0.0</v>
@@ -9209,10 +9209,10 @@
         <v>0.0</v>
       </c>
       <c r="H11">
-        <v>0.0</v>
+        <v>7.258232247011776e-15</v>
       </c>
       <c r="I11">
-        <v>1.0</v>
+        <v>1.0000000000000073</v>
       </c>
       <c r="J11">
         <v>1.0</v>
@@ -9280,7 +9280,7 @@
         <v>1.0</v>
       </c>
       <c r="E12">
-        <v>-5.5289106626332796e-14</v>
+        <v>0.0</v>
       </c>
       <c r="F12">
         <v>0.0</v>
@@ -9289,10 +9289,10 @@
         <v>0.0</v>
       </c>
       <c r="H12">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I12">
-        <v>1.7563728249569976e-13</v>
+        <v>1.0</v>
       </c>
       <c r="J12">
         <v>1.0</v>
@@ -9473,13 +9473,13 @@
         <v>1.0</v>
       </c>
       <c r="P14">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q14">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="R14">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="S14">
         <v>1.0</v>
@@ -9646,10 +9646,10 @@
         <v>59.75903614457832</v>
       </c>
       <c r="F4">
-        <v>50.0</v>
+        <v>50.00000000000001</v>
       </c>
       <c r="G4">
-        <v>50.0</v>
+        <v>50.00000000000001</v>
       </c>
       <c r="H4">
         <v>50.0</v>
@@ -9803,7 +9803,7 @@
         <v>50.0</v>
       </c>
       <c r="E6">
-        <v>55.42832979808753</v>
+        <v>55.428329798087525</v>
       </c>
       <c r="F6">
         <v>50.0</v>
@@ -9818,7 +9818,7 @@
         <v>55.428329798087525</v>
       </c>
       <c r="J6">
-        <v>61.124725265216405</v>
+        <v>61.12472526521641</v>
       </c>
       <c r="K6">
         <v>61.12472526521641</v>
@@ -9836,7 +9836,7 @@
         <v>61.12472526521641</v>
       </c>
       <c r="P6">
-        <v>61.124725265216405</v>
+        <v>61.12472526521641</v>
       </c>
       <c r="Q6">
         <v>61.12472526521641</v>
@@ -9845,7 +9845,7 @@
         <v>61.12472526521641</v>
       </c>
       <c r="S6">
-        <v>61.124725265216405</v>
+        <v>61.12472526521641</v>
       </c>
       <c r="T6">
         <v>61.12472526521641</v>
@@ -9860,10 +9860,10 @@
         <v>61.12472526521641</v>
       </c>
       <c r="X6">
-        <v>61.124725265216405</v>
+        <v>61.12472526521642</v>
       </c>
       <c r="Y6">
-        <v>61.124725265216405</v>
+        <v>61.12472526521641</v>
       </c>
       <c r="Z6">
         <v>61.12472526521641</v>
@@ -9883,7 +9883,7 @@
         <v>50.0</v>
       </c>
       <c r="E7">
-        <v>62.96767673987576</v>
+        <v>62.967676739875756</v>
       </c>
       <c r="F7">
         <v>50.0</v>
@@ -9940,7 +9940,7 @@
         <v>76.57573257801698</v>
       </c>
       <c r="X7">
-        <v>76.57573257801698</v>
+        <v>76.575732578017</v>
       </c>
       <c r="Y7">
         <v>76.57573257801698</v>
@@ -9957,13 +9957,13 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>71.41174531467857</v>
+        <v>71.41174531467858</v>
       </c>
       <c r="D8">
         <v>50.0</v>
       </c>
       <c r="E8">
-        <v>71.41174531467858</v>
+        <v>71.41174531467857</v>
       </c>
       <c r="F8">
         <v>50.0</v>
@@ -9978,16 +9978,16 @@
         <v>71.41174531467857</v>
       </c>
       <c r="J8">
-        <v>93.88086076835361</v>
+        <v>93.88086076835364</v>
       </c>
       <c r="K8">
+        <v>93.88086076835363</v>
+      </c>
+      <c r="L8">
+        <v>93.88086076835363</v>
+      </c>
+      <c r="M8">
         <v>93.88086076835364</v>
-      </c>
-      <c r="L8">
-        <v>93.88086076835364</v>
-      </c>
-      <c r="M8">
-        <v>93.88086076835363</v>
       </c>
       <c r="N8">
         <v>93.88086076835364</v>
@@ -9996,34 +9996,34 @@
         <v>93.88086076835364</v>
       </c>
       <c r="P8">
-        <v>93.88086076835361</v>
+        <v>93.88086076835364</v>
       </c>
       <c r="Q8">
-        <v>93.88086076835363</v>
+        <v>93.88086076835364</v>
       </c>
       <c r="R8">
         <v>93.88086076835364</v>
       </c>
       <c r="S8">
-        <v>93.88086076835361</v>
+        <v>93.88086076835364</v>
       </c>
       <c r="T8">
         <v>93.88086076835364</v>
       </c>
       <c r="U8">
-        <v>71.41174531467858</v>
+        <v>71.41174531467857</v>
       </c>
       <c r="V8">
         <v>93.88086076835364</v>
       </c>
       <c r="W8">
-        <v>93.88086076835364</v>
+        <v>93.88086076835363</v>
       </c>
       <c r="X8">
-        <v>93.88086076835361</v>
+        <v>93.88086076835363</v>
       </c>
       <c r="Y8">
-        <v>93.88086076835361</v>
+        <v>93.88086076835363</v>
       </c>
       <c r="Z8">
         <v>93.88086076835364</v>
@@ -10043,13 +10043,13 @@
         <v>50.0</v>
       </c>
       <c r="E9">
-        <v>80.45896164482447</v>
+        <v>80.45896164482446</v>
       </c>
       <c r="F9">
-        <v>50.0</v>
+        <v>50.00000000000003</v>
       </c>
       <c r="G9">
-        <v>50.0</v>
+        <v>50.00000000000003</v>
       </c>
       <c r="H9">
         <v>50.0</v>
@@ -10058,13 +10058,13 @@
         <v>80.45896164482446</v>
       </c>
       <c r="J9">
-        <v>112.4220695437143</v>
+        <v>112.42206954371431</v>
       </c>
       <c r="K9">
-        <v>112.42206954371431</v>
+        <v>112.42206954371433</v>
       </c>
       <c r="L9">
-        <v>112.42206954371431</v>
+        <v>112.42206954371433</v>
       </c>
       <c r="M9">
         <v>112.42206954371431</v>
@@ -10076,7 +10076,7 @@
         <v>112.42206954371431</v>
       </c>
       <c r="P9">
-        <v>112.4220695437143</v>
+        <v>112.42206954371431</v>
       </c>
       <c r="Q9">
         <v>112.42206954371431</v>
@@ -10085,7 +10085,7 @@
         <v>112.42206954371431</v>
       </c>
       <c r="S9">
-        <v>112.4220695437143</v>
+        <v>112.42206954371431</v>
       </c>
       <c r="T9">
         <v>112.42206954371431</v>
@@ -10097,13 +10097,13 @@
         <v>112.42206954371431</v>
       </c>
       <c r="W9">
+        <v>112.42206954371433</v>
+      </c>
+      <c r="X9">
         <v>112.42206954371431</v>
       </c>
-      <c r="X9">
-        <v>112.4220695437143</v>
-      </c>
       <c r="Y9">
-        <v>112.4220695437143</v>
+        <v>112.42206954371433</v>
       </c>
       <c r="Z9">
         <v>112.42206954371431</v>
@@ -10126,10 +10126,10 @@
         <v>80.0</v>
       </c>
       <c r="F10">
-        <v>50.0</v>
+        <v>50.00000000000002</v>
       </c>
       <c r="G10">
-        <v>50.0</v>
+        <v>50.00000000000002</v>
       </c>
       <c r="H10">
         <v>50.0</v>
@@ -10138,7 +10138,7 @@
         <v>80.0</v>
       </c>
       <c r="J10">
-        <v>111.48148148148147</v>
+        <v>111.48148148148148</v>
       </c>
       <c r="K10">
         <v>111.48148148148148</v>
@@ -10156,7 +10156,7 @@
         <v>111.48148148148148</v>
       </c>
       <c r="P10">
-        <v>111.48148148148147</v>
+        <v>111.48148148148148</v>
       </c>
       <c r="Q10">
         <v>111.48148148148148</v>
@@ -10165,7 +10165,7 @@
         <v>111.48148148148148</v>
       </c>
       <c r="S10">
-        <v>111.48148148148147</v>
+        <v>111.48148148148148</v>
       </c>
       <c r="T10">
         <v>111.48148148148148</v>
@@ -10180,10 +10180,10 @@
         <v>111.48148148148148</v>
       </c>
       <c r="X10">
-        <v>111.48148148148147</v>
+        <v>111.48148148148148</v>
       </c>
       <c r="Y10">
-        <v>111.48148148148147</v>
+        <v>111.48148148148148</v>
       </c>
       <c r="Z10">
         <v>111.48148148148148</v>
@@ -10206,10 +10206,10 @@
         <v>66.26506024096386</v>
       </c>
       <c r="F11">
-        <v>50.0</v>
+        <v>50.000000000000014</v>
       </c>
       <c r="G11">
-        <v>50.0</v>
+        <v>50.000000000000014</v>
       </c>
       <c r="H11">
         <v>50.0</v>
@@ -10277,28 +10277,28 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>91.08404335372745</v>
+        <v>91.08404335372747</v>
       </c>
       <c r="D12">
         <v>49.99999999999999</v>
       </c>
       <c r="E12">
-        <v>91.08404335372748</v>
+        <v>91.08404335372745</v>
       </c>
       <c r="F12">
         <v>50.0</v>
       </c>
       <c r="G12">
+        <v>50.0</v>
+      </c>
+      <c r="H12">
         <v>49.99999999999999</v>
-      </c>
-      <c r="H12">
-        <v>50.0</v>
       </c>
       <c r="I12">
         <v>91.08404335372745</v>
       </c>
       <c r="J12">
-        <v>134.19692835455254</v>
+        <v>134.19692835455257</v>
       </c>
       <c r="K12">
         <v>134.19692835455257</v>
@@ -10316,7 +10316,7 @@
         <v>134.19692835455257</v>
       </c>
       <c r="P12">
-        <v>134.19692835455254</v>
+        <v>134.19692835455257</v>
       </c>
       <c r="Q12">
         <v>134.19692835455257</v>
@@ -10325,7 +10325,7 @@
         <v>134.19692835455257</v>
       </c>
       <c r="S12">
-        <v>134.19692835455254</v>
+        <v>134.19692835455257</v>
       </c>
       <c r="T12">
         <v>134.19692835455257</v>
@@ -10340,10 +10340,10 @@
         <v>134.19692835455257</v>
       </c>
       <c r="X12">
-        <v>134.19692835455254</v>
+        <v>134.19692835455257</v>
       </c>
       <c r="Y12">
-        <v>134.19692835455254</v>
+        <v>134.19692835455257</v>
       </c>
       <c r="Z12">
         <v>134.19692835455257</v>

</xml_diff>